<commit_message>
Lagt til ekstra linje mellom bus 1 og 2
</commit_message>
<xml_diff>
--- a/prosjektfiler/System_data.xlsx
+++ b/prosjektfiler/System_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marku\Desktop\IELET2118---Prosjekt-Lastflytanalyse\prosjektfiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955AB490-D03E-4E6F-8A51-B95DA74D1376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68324DE7-C196-4A94-81AB-D66384A65952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6D3FD58-6DB6-4988-B229-9B990EF92238}"/>
   </bookViews>
@@ -770,10 +770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E81158F8-AC87-45D5-9D87-5F767982CA33}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,122 +817,122 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="6">
-        <v>3</v>
-      </c>
-      <c r="C3" s="6">
-        <v>8.3555555555555501E-3</v>
-      </c>
-      <c r="D3" s="6">
-        <v>8.9822222222222206E-2</v>
-      </c>
-      <c r="E3" s="6">
-        <v>4.6245500497903201E-3</v>
+      <c r="C3" s="5">
+        <v>1.0177777777777701E-2</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.109411111111111</v>
+      </c>
+      <c r="E3" s="5">
+        <v>5.6330955393722399E-3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
-        <v>4</v>
-      </c>
       <c r="C4" s="6">
-        <v>2.1244444444444399E-2</v>
+        <v>8.3555555555555501E-3</v>
       </c>
       <c r="D4" s="6">
-        <v>0.22837777777777701</v>
+        <v>8.9822222222222206E-2</v>
       </c>
       <c r="E4" s="6">
-        <v>1.1758164488296601E-2</v>
+        <v>4.6245500497903201E-3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
-        <v>5</v>
-      </c>
       <c r="C5" s="6">
-        <v>4.0333333333333297E-3</v>
+        <v>2.1244444444444399E-2</v>
       </c>
       <c r="D5" s="6">
-        <v>4.4366666666666603E-2</v>
+        <v>0.22837777777777701</v>
       </c>
       <c r="E5" s="6">
-        <v>3.8659496717279901E-3</v>
+        <v>1.1758164488296601E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="6">
-        <v>6</v>
-      </c>
       <c r="C6" s="6">
-        <v>1.5822222222222199E-2</v>
+        <v>4.0333333333333297E-3</v>
       </c>
       <c r="D6" s="6">
-        <v>0.25315555555555502</v>
+        <v>4.4366666666666603E-2</v>
       </c>
       <c r="E6" s="6">
-        <v>2.2949711325591801E-2</v>
+        <v>3.8659496717279901E-3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="6">
-        <v>7</v>
-      </c>
       <c r="C7" s="6">
-        <v>1.20888888888888E-2</v>
+        <v>1.5822222222222199E-2</v>
       </c>
       <c r="D7" s="6">
-        <v>0.193422222222222</v>
+        <v>0.25315555555555502</v>
       </c>
       <c r="E7" s="6">
-        <v>1.7534610900452201E-2</v>
+        <v>2.2949711325591801E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" s="6">
-        <v>8</v>
-      </c>
       <c r="C8" s="6">
-        <v>2.1955555555555499E-2</v>
+        <v>1.20888888888888E-2</v>
       </c>
       <c r="D8" s="6">
-        <v>0.23602222222222199</v>
+        <v>0.193422222222222</v>
       </c>
       <c r="E8" s="6">
-        <v>1.21517432159383E-2</v>
+        <v>1.7534610900452201E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B9" s="6">
         <v>8</v>
       </c>
       <c r="C9" s="6">
-        <v>4.7022222222222201E-2</v>
+        <v>2.1955555555555499E-2</v>
       </c>
       <c r="D9" s="6">
-        <v>0.50548888888888799</v>
+        <v>0.23602222222222199</v>
       </c>
       <c r="E9" s="6">
-        <v>2.6025393365309301E-2</v>
+        <v>1.21517432159383E-2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -940,15 +940,32 @@
         <v>1</v>
       </c>
       <c r="B10" s="6">
+        <v>8</v>
+      </c>
+      <c r="C10" s="6">
+        <v>4.7022222222222201E-2</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0.50548888888888799</v>
+      </c>
+      <c r="E10" s="6">
+        <v>2.6025393365309301E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>1</v>
+      </c>
+      <c r="B11" s="6">
         <v>6</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C11" s="6">
         <v>5.1866666666666603E-2</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D11" s="6">
         <v>0.55756666666666599</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E11" s="6">
         <v>2.8706648447368598E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Oppdatert System_data for 4d)
</commit_message>
<xml_diff>
--- a/prosjektfiler/System_data.xlsx
+++ b/prosjektfiler/System_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marku\Desktop\IELET2118---Prosjekt-Lastflytanalyse\prosjektfiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4550255-BE90-44D1-9053-2DD75B552893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76423559-61EF-47D8-9FAD-2B1AC35D92C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6D3FD58-6DB6-4988-B229-9B990EF92238}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E6D3FD58-6DB6-4988-B229-9B990EF92238}"/>
   </bookViews>
   <sheets>
     <sheet name="BranchData" sheetId="1" r:id="rId1"/>
@@ -772,7 +772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E81158F8-AC87-45D5-9D87-5F767982CA33}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
@@ -963,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C983FE4D-AF19-4D14-8B95-201C762457E9}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,7 +1218,8 @@
         <v>180</v>
       </c>
       <c r="H8" s="17">
-        <v>45</v>
+        <f>45*1.05</f>
+        <v>47.25</v>
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>

</xml_diff>